<commit_message>
mengganti rumus untuk b440
</commit_message>
<xml_diff>
--- a/app/production/compatibility_model/dashboard/result/export/data_hasil/b440_2022-09-08.xlsx
+++ b/app/production/compatibility_model/dashboard/result/export/data_hasil/b440_2022-09-08.xlsx
@@ -1206,15 +1206,19 @@
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4">
+        <f>SUM(D6:D36)</f>
         <v>2800</v>
       </c>
       <c r="E37" s="4">
+        <f>SUM(E6:E36)</f>
         <v>501</v>
       </c>
       <c r="F37" s="4">
+        <f>SUM(F6:F36)</f>
         <v>-2299</v>
       </c>
       <c r="G37" s="4">
+        <f>E37-D37</f>
         <v>-2299</v>
       </c>
     </row>

</xml_diff>